<commit_message>
Modified Output.py -- Chapter names were changed in JS but not in the Output.py, hence modified to fix bugs.
</commit_message>
<xml_diff>
--- a/app/plan/term2outcome.xlsx
+++ b/app/plan/term2outcome.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="154">
   <si>
     <r>
       <rPr>
@@ -151,7 +151,27 @@
     <t xml:space="preserve">Rhombus area</t>
   </si>
   <si>
-    <t xml:space="preserve">Geometry</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Geometry 7</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">I should know the different types of angles.</t>
@@ -184,7 +204,27 @@
     <t xml:space="preserve">Angles &amp; lines</t>
   </si>
   <si>
-    <t xml:space="preserve">Practical Geometry</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Practical Geometry 7</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">I should know angle bisector</t>
@@ -220,7 +260,27 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Algebra</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Algebra 8</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">I should be able to distinguish variables, constants, co efficient of terms and degree of expressions in an algebraic expression.</t>
@@ -404,6 +464,29 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Practical Geometry 8</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -530,6 +613,29 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Algebra 9</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="ArialMT"/>
@@ -758,6 +864,31 @@
   </si>
   <si>
     <t xml:space="preserve">Stat. measures</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Practical Geometry 9</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">I should be able to construct perpendicular bisector.</t>
@@ -823,7 +954,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -870,6 +1001,22 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -928,6 +1075,15 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -994,23 +1150,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1093,15 +1249,16 @@
   </sheetPr>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D79" activeCellId="0" sqref="D79"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="B63 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
@@ -1324,7 +1481,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
         <v>48</v>
       </c>
@@ -1360,7 +1517,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
         <v>54</v>
       </c>
@@ -1543,9 +1700,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="2" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,7 +1712,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>26</v>
@@ -1568,31 +1725,31 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C69" s="5"/>
     </row>
@@ -1603,84 +1760,84 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,18 +1847,18 @@
     </row>
     <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,15 +1868,15 @@
     </row>
     <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>96</v>
@@ -1727,15 +1884,15 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,31 +1902,31 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,23 +1936,23 @@
     </row>
     <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="8" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,10 +1962,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,18 +1975,18 @@
     </row>
     <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>